<commit_message>
Add dataset dictionary for foosball match dataset
</commit_message>
<xml_diff>
--- a/ressources/NotationHackathon.xlsx
+++ b/ressources/NotationHackathon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericp/Dev/HackathonTemplate/ressources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericp/Dev/Hackathon-Ynov/HackathonTemplate/ressources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B14F4EB-D5E0-AC4E-BF58-5AC2CA003068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01358808-783C-E842-999C-F5BBC1CB6C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" xr2:uid="{D054AFDD-6162-FD43-ADC0-80BEDE8B180E}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{D054AFDD-6162-FD43-ADC0-80BEDE8B180E}"/>
   </bookViews>
   <sheets>
     <sheet name="Grille de notation" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,6 @@
     <t>Note de groupe:</t>
   </si>
   <si>
-    <t>/50</t>
-  </si>
-  <si>
     <t>Oral Démonstration</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>/10</t>
   </si>
   <si>
-    <t>Readme final</t>
-  </si>
-  <si>
     <t>Note de département</t>
   </si>
   <si>
@@ -123,9 +117,6 @@
     <t>API Fonctionnelle</t>
   </si>
   <si>
-    <t>API Documentée (Readme/Swagger…)</t>
-  </si>
-  <si>
     <t>/2</t>
   </si>
   <si>
@@ -138,9 +129,6 @@
     <t>Gestion des erreurs (Erreurs 400/500..)</t>
   </si>
   <si>
-    <t>Gestion des rôles</t>
-  </si>
-  <si>
     <t>Lisibilité du code</t>
   </si>
   <si>
@@ -189,9 +177,6 @@
     <t>Sondage répondue</t>
   </si>
   <si>
-    <t>Travail d'équipe</t>
-  </si>
-  <si>
     <t>/20</t>
   </si>
   <si>
@@ -219,9 +204,6 @@
     <t>Schéma de BDD, cohérence avec site/dataset</t>
   </si>
   <si>
-    <t>Visualisation des données du dataset (Site, Dashboard, Playbook..)</t>
-  </si>
-  <si>
     <t>/6</t>
   </si>
   <si>
@@ -307,9 +289,6 @@
   </si>
   <si>
     <t>Captation</t>
-  </si>
-  <si>
-    <t>Capteurs pour suivre l'état des babyfoots</t>
   </si>
   <si>
     <t>Transmission</t>
@@ -411,19 +390,40 @@
     <t>L'oral présente UN PROJET dans sa globalité, pas 5 petits projets sans liens</t>
   </si>
   <si>
-    <t>Démonstration du projet global (tous les composants) de minimum 5 minutes</t>
-  </si>
-  <si>
     <t>Capacité à vulgariser, adopter une vue produit marketing</t>
   </si>
   <si>
     <t>Justification de tous les choix majeurs vulgarisés et détaillés (Boutique, Archi..)</t>
   </si>
   <si>
-    <t>Bilan d'équipe</t>
-  </si>
-  <si>
     <t>Note oral:</t>
+  </si>
+  <si>
+    <t>Projet GitHub final</t>
+  </si>
+  <si>
+    <t>Travail d'équipe (Mix aux autres départements)</t>
+  </si>
+  <si>
+    <t>/60</t>
+  </si>
+  <si>
+    <t>Démonstration du projet global (tous les composants) de minimum 3 minutes</t>
+  </si>
+  <si>
+    <t>Bilan d'équipe (diffcultés, solutions…)</t>
+  </si>
+  <si>
+    <t>API Documentée (Postman/Swagger…)</t>
+  </si>
+  <si>
+    <t>Gestion des rôles (Admin, visiteur, inscrit)</t>
+  </si>
+  <si>
+    <t>Visualisation des données du dataset (Site, Grafana, Playbook..)</t>
+  </si>
+  <si>
+    <t>Capteurs fonctionnels pour suivre l'état des babyfoots</t>
   </si>
 </sst>
 </file>
@@ -770,15 +770,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -786,15 +777,24 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1133,13 +1133,13 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="37.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" customWidth="1"/>
     <col min="3" max="3" width="4.83203125" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
     <col min="13" max="13" width="27" customWidth="1"/>
@@ -1162,17 +1162,17 @@
     </row>
     <row r="2" spans="1:13" ht="46" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -1199,105 +1199,105 @@
       <c r="B8" s="8"/>
       <c r="C8" s="8">
         <f>SUM(C9:C11)</f>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="B9" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="16">
         <f>Oral!D4</f>
         <v>30</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="19">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="B11" s="20" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="C11" s="19">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C12" s="21" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">INDIRECT("'" &amp; B12 &amp; "'!D4")</f>
         <v>25</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="23">
         <f>SUM(C14:C16)</f>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="B14" s="25" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C14" s="26">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="B15" s="28" t="s">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="C15" s="26">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="29" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C16" s="30">
         <v>2</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1322,7 +1322,7 @@
         <v>20</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1339,7 +1339,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1365,17 +1365,17 @@
     </row>
     <row r="2" spans="1:13" ht="39">
       <c r="A2" s="1"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -1384,13 +1384,13 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
+      <c r="D3" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="4" spans="1:13" ht="19">
       <c r="A4" s="13" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1408,12 +1408,12 @@
         <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="B5" s="7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7">
@@ -1421,57 +1421,57 @@
         <v>8</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="52" t="s">
-        <v>107</v>
-      </c>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
+        <v>42</v>
+      </c>
+      <c r="G5" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="5" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D6" s="5">
         <v>2</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
+        <v>17</v>
+      </c>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1">
-      <c r="C7" s="50" t="s">
-        <v>100</v>
+      <c r="C7" s="47" t="s">
+        <v>93</v>
       </c>
       <c r="D7" s="5">
         <v>3</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="C8" s="5" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D8" s="5">
         <v>3</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="B9" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9">
@@ -1479,124 +1479,124 @@
         <v>7</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="C10" s="12" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D10" s="10">
         <v>1</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="38" customHeight="1">
-      <c r="C11" s="51" t="s">
-        <v>104</v>
+      <c r="C11" s="48" t="s">
+        <v>97</v>
       </c>
       <c r="D11" s="12">
         <v>1</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="C12" s="12" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D12" s="10">
         <v>2</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="C13" s="11" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D13" s="11">
         <v>3</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="B14" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55">
+      <c r="B14" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51">
         <f>SUM(D15:D18)</f>
         <v>15</v>
       </c>
-      <c r="E14" s="54" t="s">
-        <v>109</v>
+      <c r="E14" s="50" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="52">
+        <v>4</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="17">
+      <c r="C16" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="D15" s="56">
+      <c r="D16" s="49">
         <v>4</v>
       </c>
-      <c r="E15" s="56" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="34">
-      <c r="C16" s="57" t="s">
+      <c r="E16" s="49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="C17" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="52">
+        <v>3</v>
+      </c>
+      <c r="E17" s="52" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="C18" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="49">
+        <v>4</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="C19" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="53">
-        <v>4</v>
-      </c>
-      <c r="E16" s="53" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="C17" s="53" t="s">
-        <v>112</v>
-      </c>
-      <c r="D17" s="56">
-        <v>3</v>
-      </c>
-      <c r="E17" s="56" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="C18" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" s="53">
-        <v>4</v>
-      </c>
-      <c r="E18" s="53" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="C19" s="53" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" s="53">
+      <c r="D19" s="49">
         <v>2</v>
       </c>
-      <c r="E19" s="53" t="s">
-        <v>20</v>
+      <c r="E19" s="49" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2">
@@ -1604,18 +1604,18 @@
         <v>0</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="C21" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D21" s="4">
         <v>0</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1634,7 +1634,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:E18"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1662,17 +1662,17 @@
     </row>
     <row r="2" spans="1:13" ht="39">
       <c r="A2" s="1"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -1680,14 +1680,14 @@
     <row r="3" spans="1:13">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
+      <c r="C3" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="4" spans="1:13" ht="19">
       <c r="A4" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1705,12 +1705,12 @@
         <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="B5" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7">
@@ -1718,78 +1718,78 @@
         <v>12</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5">
         <v>3</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="C7" s="5" t="s">
-        <v>19</v>
+        <v>112</v>
       </c>
       <c r="D7" s="5">
         <v>2</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="C8" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" s="5">
         <v>2</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="C9" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D9" s="5">
         <v>1</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="C10" s="5" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="D10" s="5">
         <v>2</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="C11" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D11" s="6">
         <v>2</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="B12" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9">
@@ -1797,56 +1797,56 @@
         <v>13</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="C13" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D13" s="10">
         <v>4</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="C14" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D14" s="10">
         <v>4</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="C15" s="12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D15" s="10">
         <v>3</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="C16" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D16" s="11">
         <v>2</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:12">
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2">
@@ -1854,23 +1854,23 @@
         <v>0</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:12">
       <c r="C18" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D18" s="4">
         <v>0</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:12">
       <c r="L21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1887,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E98B12-F5E5-204B-BD3E-092BFD01A3D1}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="115" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView zoomScale="115" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1914,17 +1914,17 @@
     </row>
     <row r="2" spans="1:13" ht="39">
       <c r="A2" s="1"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -1932,14 +1932,14 @@
     <row r="3" spans="1:13">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="47" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
+      <c r="C3" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1948,7 +1948,7 @@
     </row>
     <row r="4" spans="1:13" ht="19">
       <c r="A4" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1957,12 +1957,12 @@
         <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="B5" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7">
@@ -1970,45 +1970,45 @@
         <v>6</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D6" s="5">
         <v>2</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="C7" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D7" s="5">
         <v>2</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="C8" s="6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D8" s="6">
         <v>2</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="B9" s="37" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C9" s="37"/>
       <c r="D9" s="37">
@@ -2016,34 +2016,34 @@
         <v>6</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="C10" s="43" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D10" s="43">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="C11" s="39" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D11" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" s="39" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="B12" s="23" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="23">
@@ -2051,45 +2051,45 @@
         <v>5</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="C13" s="44" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D13" s="44">
         <v>2</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="C14" s="44" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D14" s="44">
         <v>2</v>
       </c>
       <c r="E14" s="44" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="C15" s="45" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D15" s="45">
         <v>1</v>
       </c>
       <c r="E15" s="45" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="8" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8">
@@ -2097,45 +2097,45 @@
         <v>8</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="C17" s="12" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D17" s="12">
         <v>3</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:5">
       <c r="C18" s="12" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D18" s="12">
         <v>3</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:5">
       <c r="C19" s="11" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D19" s="11">
         <v>2</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2">
@@ -2143,29 +2143,29 @@
         <v>0</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="C21" s="42" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D21" s="42">
         <v>0</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="2:5">
       <c r="C22" s="42" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D22" s="42">
         <v>0</v>
       </c>
       <c r="E22" s="42" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2181,8 +2181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE06351-FF09-734B-AAA1-1FF5290E74E9}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="137" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2214,12 +2214,12 @@
     </row>
     <row r="2" spans="1:13" ht="39">
       <c r="A2" s="1"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
       <c r="F2" s="38"/>
       <c r="G2" s="38"/>
       <c r="H2" s="38"/>
@@ -2232,10 +2232,10 @@
     <row r="3" spans="1:13">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="48"/>
+      <c r="C3" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="57"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -2248,7 +2248,7 @@
     </row>
     <row r="4" spans="1:13" ht="19">
       <c r="A4" s="33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="32"/>
       <c r="C4" s="2"/>
@@ -2257,12 +2257,12 @@
         <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="B5" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7">
@@ -2270,56 +2270,56 @@
         <v>12</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="34" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D6" s="34">
         <v>5</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="C7" s="34" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D7" s="34">
         <v>3</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="C8" s="35" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D8" s="35">
         <v>2</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="C9" s="35" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D9" s="35">
         <v>2</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="37" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C10" s="37"/>
       <c r="D10" s="37">
@@ -2327,34 +2327,34 @@
         <v>7</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="C11" s="36" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D11" s="36">
         <v>2</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="C12" s="39" t="s">
-        <v>51</v>
+        <v>114</v>
       </c>
       <c r="D12" s="39">
         <v>5</v>
       </c>
       <c r="E12" s="39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="B13" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8">
@@ -2362,45 +2362,45 @@
         <v>6</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="C14" s="40" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D14" s="40">
         <v>2</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="C15" s="12" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D15" s="12">
         <v>2</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="C16" s="11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D16" s="11">
         <v>2</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2">
@@ -2408,29 +2408,29 @@
         <v>0</v>
       </c>
       <c r="E17" s="41" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:5">
       <c r="C18" s="42" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D18" s="42">
         <v>0</v>
       </c>
       <c r="E18" s="42" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="2:5">
       <c r="C19" s="42" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D19" s="42">
         <v>0</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2447,7 +2447,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="137" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2479,12 +2479,12 @@
     </row>
     <row r="2" spans="1:13" ht="39">
       <c r="A2" s="1"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
       <c r="F2" s="38"/>
       <c r="G2" s="38"/>
       <c r="H2" s="38"/>
@@ -2497,10 +2497,10 @@
     <row r="3" spans="1:13">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="48"/>
+      <c r="C3" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="57"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -2513,21 +2513,21 @@
     </row>
     <row r="4" spans="1:13" ht="19">
       <c r="A4" s="33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="32"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2">
         <f>SUM(D5,D9,D13)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="B5" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7">
@@ -2535,45 +2535,45 @@
         <v>10</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="34" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="D6" s="34">
         <v>4</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="C7" s="34" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D7" s="34">
         <v>3</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="C8" s="35" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D8" s="35">
         <v>3</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="B9" s="37" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C9" s="37"/>
       <c r="D9" s="37">
@@ -2581,80 +2581,80 @@
         <v>10</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="C10" s="36" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D10" s="36">
         <v>5</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="C11" s="39" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D11" s="39">
         <v>3</v>
       </c>
       <c r="E11" s="39" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="C12" s="39" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D12" s="39">
         <v>2</v>
       </c>
       <c r="E12" s="39" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="B13" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8">
         <f>SUM(D14:D15)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="C14" s="40" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D14" s="40">
         <v>3</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="C15" s="12" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D15" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2">
@@ -2662,18 +2662,18 @@
         <v>0</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="3:5">
-      <c r="C17" s="49" t="s">
-        <v>36</v>
+      <c r="C17" s="46" t="s">
+        <v>32</v>
       </c>
       <c r="D17" s="42">
         <v>0</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2690,7 +2690,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="137" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2722,12 +2722,12 @@
     </row>
     <row r="2" spans="1:13" ht="39">
       <c r="A2" s="1"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
       <c r="F2" s="38"/>
       <c r="G2" s="38"/>
       <c r="H2" s="38"/>
@@ -2740,10 +2740,10 @@
     <row r="3" spans="1:13">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="48"/>
+      <c r="C3" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="57"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -2756,7 +2756,7 @@
     </row>
     <row r="4" spans="1:13" ht="19">
       <c r="A4" s="33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="32"/>
       <c r="C4" s="2"/>
@@ -2765,12 +2765,12 @@
         <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="B5" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7">
@@ -2778,45 +2778,45 @@
         <v>13</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="34" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D6" s="34">
         <v>5</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="C7" s="34" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D7" s="34">
         <v>4</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="C8" s="34" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D8" s="34">
         <v>4</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="B9" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8">
@@ -2824,45 +2824,45 @@
         <v>12</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="C10" s="40" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D10" s="40">
         <v>4</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="C11" s="40" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D11" s="40">
         <v>4</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="C12" s="12" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D12" s="12">
         <v>4</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="B13" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2">
@@ -2870,18 +2870,18 @@
         <v>0</v>
       </c>
       <c r="E13" s="41" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="C14" s="49" t="s">
-        <v>36</v>
+      <c r="C14" s="46" t="s">
+        <v>32</v>
       </c>
       <c r="D14" s="42">
         <v>0</v>
       </c>
       <c r="E14" s="42" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update NotationHackathon.xlsx with revised data
</commit_message>
<xml_diff>
--- a/ressources/NotationHackathon.xlsx
+++ b/ressources/NotationHackathon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericp/Dev/Hackathon-Ynov/HackathonTemplate/ressources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01358808-783C-E842-999C-F5BBC1CB6C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F00C93-6A30-E348-9548-591D3C03B32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{D054AFDD-6162-FD43-ADC0-80BEDE8B180E}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" activeTab="1" xr2:uid="{D054AFDD-6162-FD43-ADC0-80BEDE8B180E}"/>
   </bookViews>
   <sheets>
     <sheet name="Grille de notation" sheetId="1" r:id="rId1"/>
@@ -1132,7 +1132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19A7D134-824F-1D45-BFDC-F17802F9F10C}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+    <sheetView zoomScale="107" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1338,8 +1338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5930D84F-E2CE-B544-AAD5-2EA1D34C843F}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1532,7 +1532,7 @@
       </c>
       <c r="C14" s="51"/>
       <c r="D14" s="51">
-        <f>SUM(D15:D18)</f>
+        <f>SUM(D15:D19)</f>
         <v>15</v>
       </c>
       <c r="E14" s="50" t="s">
@@ -1566,10 +1566,10 @@
         <v>104</v>
       </c>
       <c r="D17" s="52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="2:5">
@@ -1577,10 +1577,10 @@
         <v>105</v>
       </c>
       <c r="D18" s="49">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E18" s="49" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:5">

</xml_diff>